<commit_message>
AddReservation Method is optimized.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -8,7 +8,6 @@
     <sheet state="visible" name="ReceivePayment" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="CashPayment" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="UpdateReservation" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="CheckInKeyIn" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -24,6 +23,12 @@
     <t>confirmation Number</t>
   </si>
   <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
     <t>Prepaid Or Partial</t>
   </si>
   <si>
@@ -45,7 +50,7 @@
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP456100</t>
+    <t>CHAP456400</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
@@ -120,7 +125,7 @@
     <t>Email Id</t>
   </si>
   <si>
-    <t>BRHM1166048</t>
+    <t>BRHM1166143</t>
   </si>
   <si>
     <t>Card</t>
@@ -142,7 +147,7 @@
     </r>
   </si>
   <si>
-    <t>BRHM1166047</t>
+    <t>BRHM1166144</t>
   </si>
   <si>
     <t>Cash</t>
@@ -152,22 +157,17 @@
   </si>
   <si>
     <t>Update Reservation</t>
-  </si>
-  <si>
-    <t>BRHM1166045</t>
-  </si>
-  <si>
-    <t>Check In / Key In</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d-mmm"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="d-mmm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -175,9 +175,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF22191B"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="9.0"/>
@@ -185,18 +194,14 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF22191B"/>
-      <name val="Monospace"/>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -219,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -229,26 +234,41 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -275,10 +295,6 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -488,7 +504,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="33.5"/>
     <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="17.25"/>
+    <col customWidth="1" min="3" max="5" width="17.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,10 +514,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -516,21 +532,27 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="4">
+        <v>45761.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45761.0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -541,6 +563,12 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -559,72 +587,90 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8">
+        <v>45761.0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>45761.0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45761.0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45761.0</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -649,55 +695,55 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>33</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="7">
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="11">
         <v>45927.0</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="12">
         <v>686.0</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="8">
+      <c r="F2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="12">
         <v>30048.0</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>38</v>
+      <c r="H2" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -719,19 +765,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>27</v>
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>40</v>
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -754,52 +800,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="20.63"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testNG.xml File is added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -5,12 +5,13 @@
   <sheets>
     <sheet state="visible" name="ThirdParty" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="KodaWalkIn" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="SearchThirdParty" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="CashPayment" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CardPayment" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="CheckinCard" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="CheckinCash" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="UpdateReservation" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Sheet29" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="SearchThirdParty" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="CashPayment" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="CardPayment" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="CheckinCard" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="CheckinCash" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="UpdateReservation" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
   <si>
     <t>Select Source</t>
   </si>
@@ -50,10 +51,13 @@
     <t>State</t>
   </si>
   <si>
+    <t>Oversize Category</t>
+  </si>
+  <si>
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP451006</t>
+    <t>CHAP451018</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
@@ -68,16 +72,19 @@
     <t>Avalon</t>
   </si>
   <si>
-    <t>Il75407</t>
+    <t>Il75408</t>
   </si>
   <si>
     <t>Illinois</t>
   </si>
   <si>
+    <t>Medium - $5.00</t>
+  </si>
+  <si>
     <t>AirportParking</t>
   </si>
   <si>
-    <t>AP457871006</t>
+    <t>AP457871016</t>
   </si>
   <si>
     <t>Blue</t>
@@ -95,10 +102,13 @@
     <t>Tennessee</t>
   </si>
   <si>
+    <t>Large - $7.00</t>
+  </si>
+  <si>
     <t>GlobalParkingReservation</t>
   </si>
   <si>
-    <t>GPR7891006</t>
+    <t>GPR7891012</t>
   </si>
   <si>
     <t>Maroon</t>
@@ -116,6 +126,9 @@
     <t>South Dakota</t>
   </si>
   <si>
+    <t>ExtraLarge - $9.00</t>
+  </si>
+  <si>
     <t>Reservation Prepaid</t>
   </si>
   <si>
@@ -125,7 +138,7 @@
     <t>Non Prepaid</t>
   </si>
   <si>
-    <t>NC45769</t>
+    <t>NC45761</t>
   </si>
   <si>
     <t>North Carolina</t>
@@ -161,7 +174,7 @@
     <t>Arizona</t>
   </si>
   <si>
-    <t>CHAP451005</t>
+    <t>CHAP451015</t>
   </si>
   <si>
     <t>Confirmation Number</t>
@@ -170,7 +183,7 @@
     <t>PaymentMode</t>
   </si>
   <si>
-    <t>AP457871005</t>
+    <t>BRHM1166391</t>
   </si>
   <si>
     <t>Cash</t>
@@ -198,6 +211,9 @@
   </si>
   <si>
     <t>Phone Number</t>
+  </si>
+  <si>
+    <t>BRHM1166394</t>
   </si>
   <si>
     <t>Card</t>
@@ -219,7 +235,7 @@
     </r>
   </si>
   <si>
-    <t>BRHM1166316</t>
+    <t>BRHM1166392</t>
   </si>
   <si>
     <t>Billa</t>
@@ -235,19 +251,19 @@
     </r>
   </si>
   <si>
-    <t>BRHM1166287</t>
+    <t>BRHM1166395</t>
   </si>
   <si>
     <t>Test@example.com</t>
   </si>
   <si>
-    <t>BRHM1166286</t>
+    <t>BRHM1166396</t>
   </si>
   <si>
     <t>Test2@example.com</t>
   </si>
   <si>
-    <t>BRHM1166282</t>
+    <t>AP457871011</t>
   </si>
   <si>
     <t>Click Button</t>
@@ -282,14 +298,14 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9.0"/>
       <color rgb="FF22191B"/>
       <name val="Monospace"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -341,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -354,14 +370,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -377,6 +393,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -457,6 +476,10 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -700,101 +723,113 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>45767.0</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45769.0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45769.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45769.0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45769.0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45767.0</v>
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45769.0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45769.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>31</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>5</v>
@@ -843,89 +878,89 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>45767.0</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45769.0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45769.0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>45767.0</v>
+        <v>41</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45769.0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45769.0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="4">
-        <v>45767.0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45767.0</v>
+        <v>37</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45768.0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45768.0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -934,6 +969,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -953,7 +1002,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -961,7 +1010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -973,144 +1022,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>51</v>
+      <c r="A2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="17.13"/>
-    <col customWidth="1" min="2" max="2" width="18.0"/>
-    <col customWidth="1" min="3" max="3" width="17.63"/>
-    <col customWidth="1" min="4" max="4" width="19.75"/>
-    <col customWidth="1" min="10" max="10" width="19.13"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="14">
-        <v>45927.0</v>
-      </c>
-      <c r="E2" s="15">
-        <v>686.0</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="15">
-        <v>30048.0</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="18">
-        <v>4.177760725E9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="14">
-        <v>45927.0</v>
-      </c>
-      <c r="E3" s="15">
-        <v>686.0</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="15">
-        <v>30048.0</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="18">
-        <v>4.157750825E9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="H2"/>
-    <hyperlink r:id="rId2" ref="H3"/>
-  </hyperlinks>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1132,98 +1059,220 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>59</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="15">
+        <v>45927.0</v>
+      </c>
+      <c r="E2" s="16">
+        <v>686.0</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="21">
-        <v>45927.0</v>
-      </c>
-      <c r="E2" s="22">
-        <v>111.0</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="22">
-        <v>23455.0</v>
-      </c>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="16">
+        <v>30048.0</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="23" t="b">
+      <c r="I2" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="24">
-        <v>4.087873645E9</v>
+      <c r="J2" s="19">
+        <v>4.177760725E9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="15">
+        <v>45927.0</v>
+      </c>
+      <c r="E3" s="16">
+        <v>686.0</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="16">
+        <v>30048.0</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19">
+        <v>4.157750825E9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="H2"/>
+    <hyperlink r:id="rId2" ref="H3"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.13"/>
+    <col customWidth="1" min="2" max="2" width="18.0"/>
+    <col customWidth="1" min="3" max="3" width="17.63"/>
+    <col customWidth="1" min="4" max="4" width="19.75"/>
+    <col customWidth="1" min="10" max="10" width="19.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="H1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="21">
+      <c r="I1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="22">
         <v>45927.0</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E2" s="23">
         <v>111.0</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="23">
+        <v>23455.0</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="25">
+        <v>4.087873645E9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="22">
+      <c r="C3" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="22">
+        <v>45927.0</v>
+      </c>
+      <c r="E3" s="23">
+        <v>111.0</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="23">
         <v>48767.0</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="23" t="b">
+      <c r="H3" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="25">
         <v>4.080873645E9</v>
       </c>
     </row>
@@ -1232,7 +1281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1243,19 +1292,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="25" t="s">
-        <v>48</v>
+      <c r="A1" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1263,7 +1312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1282,15 +1331,15 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>